<commit_message>
cleaning SOLD bib file
</commit_message>
<xml_diff>
--- a/Papers/HDL - A Harmonised Dataset Model for Linked Data/tables/Harmonised Dataset Model.xlsx
+++ b/Papers/HDL - A Harmonised Dataset Model for Linked Data/tables/Harmonised Dataset Model.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25703"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadassaf/Google Drive/PhD TelecomParisTech - EURECOM - France 2012-2015/My PhD Documents/Papers/HDL - A Harmonised Dataset Model for Linked Data/tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19160" yWindow="0" windowWidth="19160" windowHeight="23540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="19240" yWindow="460" windowWidth="19160" windowHeight="23540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="231">
   <si>
     <t>Label</t>
   </si>
@@ -494,13 +499,232 @@
   </si>
   <si>
     <t>https://lists.okfn.org/pipermail/ckan-dev/2013-November/006238.html</t>
+  </si>
+  <si>
+    <t>POD</t>
+  </si>
+  <si>
+    <t>DCAT</t>
+  </si>
+  <si>
+    <t>VoID</t>
+  </si>
+  <si>
+    <t>Schema.org</t>
+  </si>
+  <si>
+    <t>dc:title</t>
+  </si>
+  <si>
+    <t>dct:description</t>
+  </si>
+  <si>
+    <t>CKAN, DKAN</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>dct:modified</t>
+  </si>
+  <si>
+    <t>dateModified</t>
+  </si>
+  <si>
+    <t>isPartOf</t>
+  </si>
+  <si>
+    <t>systemOfRecords</t>
+  </si>
+  <si>
+    <t>primaryITInvestmentUII</t>
+  </si>
+  <si>
+    <t>describedBy</t>
+  </si>
+  <si>
+    <t>describedByType</t>
+  </si>
+  <si>
+    <t>conformsTo</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>dct:license</t>
+  </si>
+  <si>
+    <t>dct:identifier</t>
+  </si>
+  <si>
+    <t>contactPoint:hasEmail</t>
+  </si>
+  <si>
+    <t>dcat:contactPoint-&gt;vcard:hasEmail</t>
+  </si>
+  <si>
+    <t>provider-&gt;person:email</t>
+  </si>
+  <si>
+    <t>contactPoint:fn</t>
+  </si>
+  <si>
+    <t>dcat:contactPoint-&gt;vcard:fn</t>
+  </si>
+  <si>
+    <t>provider-&gt;person:name</t>
+  </si>
+  <si>
+    <t>bureauCode</t>
+  </si>
+  <si>
+    <t>programCode</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>dcat:distribution</t>
+  </si>
+  <si>
+    <t>dct:rights</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>theme</t>
+  </si>
+  <si>
+    <t>dcat:theme</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>dataQuality</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>dct:language</t>
+  </si>
+  <si>
+    <t>inLanguage</t>
+  </si>
+  <si>
+    <t>accuralPeriodicity</t>
+  </si>
+  <si>
+    <t>dct:accuralPeriodicity</t>
+  </si>
+  <si>
+    <t>dct:issued</t>
+  </si>
+  <si>
+    <t>datePublished</t>
+  </si>
+  <si>
+    <t>dct:temporal</t>
+  </si>
+  <si>
+    <t>dct:spatial</t>
+  </si>
+  <si>
+    <t>dct:publisher-&gt;foat:name</t>
+  </si>
+  <si>
+    <t>publisher-&gt;organization:name</t>
+  </si>
+  <si>
+    <t>dct:publisher-&gt;org:subOrganizationOf</t>
+  </si>
+  <si>
+    <t>publisher-&gt;organization:memberOf</t>
+  </si>
+  <si>
+    <t>landingPage</t>
+  </si>
+  <si>
+    <t>dcat:landingPage</t>
+  </si>
+  <si>
+    <t>dct:references</t>
+  </si>
+  <si>
+    <t>subOrganizationOf</t>
+  </si>
+  <si>
+    <t>downloadURL</t>
+  </si>
+  <si>
+    <t>dcat:accessURL</t>
+  </si>
+  <si>
+    <t>contentURL</t>
+  </si>
+  <si>
+    <t>accessURL</t>
+  </si>
+  <si>
+    <t>dcat:downloadURL</t>
+  </si>
+  <si>
+    <t>mediaType</t>
+  </si>
+  <si>
+    <t>dcat:mediaType</t>
+  </si>
+  <si>
+    <t>dct:format</t>
+  </si>
+  <si>
+    <t>encodingFormat</t>
+  </si>
+  <si>
+    <t>dct:title</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>language is available on the dataset level, however it can be more suitable to have it on the resource level like the extension of CKAN model in: https://www.govdata.de/</t>
+  </si>
+  <si>
+    <t>ratings_average (govdata.de)</t>
+  </si>
+  <si>
+    <t>temporal_coverage_to</t>
+  </si>
+  <si>
+    <t>temporal_granularity</t>
+  </si>
+  <si>
+    <t>temporal_coverage_from</t>
+  </si>
+  <si>
+    <t>attribution_text</t>
+  </si>
+  <si>
+    <t>spatial-text</t>
+  </si>
+  <si>
+    <t>geographical_granularity</t>
+  </si>
+  <si>
+    <t>subgroups</t>
+  </si>
+  <si>
+    <t>dct:keyword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -555,6 +779,35 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -573,7 +826,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -603,8 +856,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -617,11 +882,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -649,11 +924,28 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -981,11 +1273,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5" bestFit="1" customWidth="1"/>
@@ -993,7 +1285,7 @@
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1302,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1027,7 +1319,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1044,7 +1336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1061,7 +1353,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1073,7 +1365,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1375,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="18">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1093,7 +1385,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="18">
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1107,7 +1399,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18">
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1121,7 +1413,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18">
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1135,7 +1427,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18">
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1149,7 +1441,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -1159,7 +1451,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="18">
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1171,7 +1463,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18">
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -1183,7 +1475,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18">
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1195,7 +1487,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18">
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -1207,7 +1499,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18">
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -1217,7 +1509,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="18">
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -1231,7 +1523,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18">
+    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -1243,7 +1535,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18">
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
@@ -1257,7 +1549,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18">
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1271,7 +1563,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18">
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1285,32 +1577,32 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -1318,32 +1610,32 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -1351,17 +1643,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1369,47 +1661,47 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>92</v>
       </c>
@@ -1417,12 +1709,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -1430,47 +1722,47 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>157</v>
       </c>
@@ -1510,30 +1802,28 @@
     <hyperlink ref="D22" r:id="rId28" location="issued"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.1640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>101</v>
       </c>
@@ -1543,15 +1833,27 @@
       <c r="C1" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="7" t="s">
+      <c r="D1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" ht="18">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1560,18 +1862,27 @@
       <c r="C3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="18">
-      <c r="A4" s="8"/>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
       <c r="B4" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="18">
-      <c r="A5" s="8"/>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
       <c r="B5" s="4" t="s">
         <v>106</v>
       </c>
@@ -1579,8 +1890,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18">
-      <c r="A6" s="8"/>
+    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
       <c r="B6" s="4" t="s">
         <v>107</v>
       </c>
@@ -1588,8 +1899,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18">
-      <c r="A7" s="8"/>
+    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
       <c r="B7" s="4" t="s">
         <v>75</v>
       </c>
@@ -1597,563 +1908,977 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18">
-      <c r="A8" s="8"/>
+    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
       <c r="B8" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18">
-      <c r="A9" s="8"/>
+    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
       <c r="B9" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="18">
-      <c r="A10" s="8"/>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
       <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="18">
-      <c r="A11" s="8"/>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
       <c r="B11" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18">
-      <c r="A12" s="8"/>
+    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
       <c r="B12" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="D13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>201</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D19" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D20" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D21" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D22" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D23" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D24" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D25" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" t="s">
+        <v>194</v>
+      </c>
+      <c r="G25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D26" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="18">
-      <c r="A14" s="8"/>
-      <c r="B14" s="4" t="s">
+      <c r="D27" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>175</v>
+      </c>
+      <c r="G27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="18">
-      <c r="A15" s="8"/>
-      <c r="B15" s="4" t="s">
+    <row r="29" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18">
-      <c r="A16" s="8"/>
-      <c r="B16" s="4" t="s">
+    <row r="30" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C30" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="18">
-      <c r="A17" s="8" t="s">
+      <c r="D30" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="4"/>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="4"/>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18">
-      <c r="A18" s="8"/>
-      <c r="B18" s="4" t="s">
+    <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18">
-      <c r="A19" s="8"/>
-      <c r="B19" s="4" t="s">
+    <row r="36" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18">
-      <c r="A20" s="8"/>
-      <c r="B20" s="4" t="s">
+    <row r="37" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18">
-      <c r="A21" s="8"/>
-      <c r="B21" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="18">
-      <c r="A22" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="18">
-      <c r="A23" s="8"/>
-      <c r="B23" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18">
-      <c r="A24" s="8"/>
-      <c r="B24" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="18">
-      <c r="A25" s="8"/>
-      <c r="B25" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="18">
-      <c r="A26" s="8"/>
-      <c r="B26" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="18">
-      <c r="A27" s="8"/>
-      <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="18">
-      <c r="A28" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" ht="18">
-      <c r="A29" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="18">
-      <c r="A30" s="8"/>
-      <c r="B30" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="18">
-      <c r="A31" s="8"/>
-      <c r="B31" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="18">
-      <c r="A32" s="8"/>
-      <c r="B32" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18">
-      <c r="A33" s="8"/>
-      <c r="B33" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="18">
-      <c r="A34" s="8"/>
-      <c r="B34" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="18">
-      <c r="A35" s="8"/>
-      <c r="B35" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="18">
-      <c r="A36" s="8"/>
-      <c r="B36" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="18">
-      <c r="A37" s="8"/>
-      <c r="B37" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="18">
-      <c r="A38" s="8" t="s">
-        <v>126</v>
-      </c>
+    <row r="38" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
       <c r="B38" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="18">
-      <c r="A39" s="8"/>
-      <c r="B39" s="4" t="s">
+      <c r="C38" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" t="s">
+        <v>198</v>
+      </c>
+      <c r="G40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E42" t="s">
+        <v>181</v>
+      </c>
+      <c r="G42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
+        <v>177</v>
+      </c>
+      <c r="E43" t="s">
+        <v>178</v>
+      </c>
+      <c r="G43" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" s="10"/>
+    </row>
+    <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" t="s">
+        <v>202</v>
+      </c>
+      <c r="G51" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="B52" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="B53" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="4"/>
+      <c r="D60" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" t="s">
+        <v>204</v>
+      </c>
+      <c r="G60" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="B62" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="18">
-      <c r="A40" s="7" t="s">
+    <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" spans="1:3" ht="18">
-      <c r="A41" s="8" t="s">
+      <c r="B63" s="10"/>
+    </row>
+    <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="18">
-      <c r="A42" s="8"/>
-      <c r="B42" s="4" t="s">
+    <row r="65" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C65" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="18">
-      <c r="A43" s="8"/>
-      <c r="B43" s="4" t="s">
+    <row r="66" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+      <c r="B66" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="18">
-      <c r="A44" s="8"/>
-      <c r="B44" s="4" t="s">
+    <row r="67" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A67" s="11"/>
+      <c r="B67" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18">
-      <c r="A45" s="8"/>
-      <c r="B45" s="4" t="s">
+    <row r="68" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="18">
-      <c r="A46" s="8"/>
-      <c r="B46" s="4" t="s">
+    <row r="69" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+      <c r="B69" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="18">
-      <c r="A47" s="8"/>
-      <c r="B47" s="4" t="s">
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>163</v>
+      </c>
+      <c r="G69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+      <c r="B70" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="18">
-      <c r="A48" s="8"/>
-      <c r="B48" s="4" t="s">
+      <c r="D70" t="s">
+        <v>125</v>
+      </c>
+      <c r="E70" t="s">
+        <v>217</v>
+      </c>
+      <c r="G70" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A71" s="11"/>
+      <c r="B71" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A72" s="11"/>
+      <c r="B72" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="18">
-      <c r="A49" s="8"/>
-      <c r="B49" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="18">
-      <c r="A50" s="8"/>
-      <c r="B50" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="18">
-      <c r="A51" s="8"/>
-      <c r="B51" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="18">
-      <c r="A52" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="18">
-      <c r="A53" s="8"/>
-      <c r="B53" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="18">
-      <c r="A54" s="8"/>
-      <c r="B54" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="18">
-      <c r="A55" s="8"/>
-      <c r="B55" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="18">
-      <c r="A56" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="18">
-      <c r="A57" s="8"/>
-      <c r="B57" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="18">
-      <c r="A58" s="8"/>
-      <c r="B58" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="18">
-      <c r="A59" s="8"/>
-      <c r="B59" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="18">
-      <c r="A60" s="8"/>
-      <c r="B60" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="18">
-      <c r="A61" s="8"/>
-      <c r="B61" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="18">
-      <c r="A62" s="8"/>
-      <c r="B62" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="18">
-      <c r="A63" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B63" s="7"/>
-    </row>
-    <row r="64" spans="1:3" ht="18">
-      <c r="A64" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="18">
-      <c r="A65" s="8"/>
-      <c r="B65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="18">
-      <c r="A66" s="8"/>
-      <c r="B66" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="18">
-      <c r="A67" s="8"/>
-      <c r="B67" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="18">
-      <c r="A68" s="8"/>
-      <c r="B68" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="18">
-      <c r="A69" s="8"/>
-      <c r="B69" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="18">
-      <c r="A70" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B70" s="7"/>
-    </row>
-    <row r="71" spans="1:3" ht="18">
-      <c r="A71" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="18">
-      <c r="A72" s="8"/>
-      <c r="B72" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="18">
-      <c r="A73" s="8"/>
+    <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A73" s="11"/>
       <c r="B73" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="18">
-      <c r="A74" s="8"/>
+      <c r="D73" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" t="s">
+        <v>219</v>
+      </c>
+      <c r="G73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A74" s="11"/>
       <c r="B74" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="11"/>
+      <c r="B75" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A76" s="11"/>
+      <c r="B76" s="4"/>
+      <c r="D76" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A77" s="11"/>
+      <c r="B77" s="4"/>
+      <c r="D77" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A78" s="11"/>
+      <c r="B78" s="4"/>
+      <c r="D78" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A80" s="11"/>
+      <c r="B80" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A81" s="11"/>
+      <c r="B81" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C81" t="s">
+        <v>109</v>
+      </c>
+      <c r="D81" t="s">
+        <v>210</v>
+      </c>
+      <c r="E81" t="s">
+        <v>214</v>
+      </c>
+      <c r="G81" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A82" s="11"/>
+      <c r="B82" s="4"/>
+      <c r="D82" t="s">
+        <v>213</v>
+      </c>
+      <c r="E82" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A83" s="11"/>
+      <c r="B83" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A85" s="11"/>
+      <c r="B85" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A86" s="11"/>
+      <c r="B86" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" s="11"/>
+      <c r="B87" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" s="11"/>
+      <c r="B88" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A89" s="11"/>
+      <c r="B89" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+    </row>
+    <row r="91" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="10"/>
+    </row>
+    <row r="92" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A92" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A93" s="11"/>
+      <c r="B93" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A94" s="11"/>
+      <c r="B94" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A95" s="11"/>
+      <c r="B95" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A96" s="11"/>
+      <c r="B96" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A97" s="11"/>
+      <c r="B97" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A98" s="11"/>
+      <c r="B98" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99" s="10"/>
+    </row>
+    <row r="100" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A100" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A101" s="11"/>
+      <c r="B101" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A102" s="11"/>
+      <c r="B102" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A103" s="11"/>
+      <c r="B103" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="18">
-      <c r="A75" s="8"/>
-      <c r="B75" s="4" t="s">
+    <row r="104" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A104" s="11"/>
+      <c r="B104" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C104" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="18">
-      <c r="A76" s="6" t="s">
+    <row r="105" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>114</v>
       </c>
     </row>
+    <row r="108" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A109" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" t="s">
+        <v>230</v>
+      </c>
+      <c r="D109" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B110" t="s">
+        <v>52</v>
+      </c>
+      <c r="C110" t="s">
+        <v>186</v>
+      </c>
+      <c r="D110" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B111" t="s">
+        <v>189</v>
+      </c>
+      <c r="C111" t="s">
+        <v>190</v>
+      </c>
+      <c r="D111" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B112" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B113" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:A69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:A75"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:A51"/>
-    <mergeCell ref="A52:A55"/>
+  <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>